<commit_message>
add fundamental factor parameters
</commit_message>
<xml_diff>
--- a/config/factorTable2023.xlsx
+++ b/config/factorTable2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramFiles\python\strategy_factor\BigMom2023\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE27343-47B3-4A7A-B268-BE27191A7154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4451DC3-94BA-42EF-A204-07AF34DEE2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42300" yWindow="3885" windowWidth="21330" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38985" yWindow="4680" windowWidth="21330" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="340">
   <si>
     <t>formula</t>
   </si>
@@ -1220,7 +1220,99 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>str('D:/Data/tushare/factor/spot_price.csv');list((5, 10, 20, 30, 60));list((10,5))</t>
+    <t>alpha_f2</t>
+  </si>
+  <si>
+    <t>alpha_f3</t>
+  </si>
+  <si>
+    <t>alpha_f4</t>
+  </si>
+  <si>
+    <t>alpha_f5</t>
+  </si>
+  <si>
+    <t>alpha_f6</t>
+  </si>
+  <si>
+    <t>alpha_f7</t>
+  </si>
+  <si>
+    <t>alpha_f8</t>
+  </si>
+  <si>
+    <t>alpha_f9</t>
+  </si>
+  <si>
+    <t>spot_basis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_sub_spread</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>oi_all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio5_w</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio10_w</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ls_ratio_w</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/spot_basis.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/main_sub_spread.csv');list((5,20,60,90,120));list((1,5,10,15,21))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/oi_all.csv');list((5,20,60,90,120));list((1,5,10,15,22))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate.csv');list((5,20,60,90,120));list((1,5,10,15,23))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,24))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,25))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate.csv');list((5,20,60,90,120));list((1,5,10,15,24))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,25))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,26))</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1303,7 +1395,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1610,22 +1702,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H222"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C216" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B212" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G222" sqref="G222"/>
+      <selection pane="bottomRight" activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.375" customWidth="1"/>
-    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.25" customWidth="1"/>
+    <col min="3" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="17.875" customWidth="1"/>
     <col min="7" max="7" width="86.375" customWidth="1"/>
     <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
@@ -6144,6 +6235,9 @@
       <c r="A222" s="2" t="s">
         <v>312</v>
       </c>
+      <c r="B222" t="s">
+        <v>322</v>
+      </c>
       <c r="E222">
         <v>2</v>
       </c>
@@ -6151,7 +6245,143 @@
         <v>313</v>
       </c>
       <c r="G222" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A223" s="2" t="s">
         <v>314</v>
+      </c>
+      <c r="B223" t="s">
+        <v>323</v>
+      </c>
+      <c r="E223">
+        <v>2</v>
+      </c>
+      <c r="F223" t="s">
+        <v>313</v>
+      </c>
+      <c r="G223" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A224" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B224" t="s">
+        <v>324</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+      <c r="F224" t="s">
+        <v>313</v>
+      </c>
+      <c r="G224" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A225" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B225" t="s">
+        <v>325</v>
+      </c>
+      <c r="E225">
+        <v>2</v>
+      </c>
+      <c r="F225" t="s">
+        <v>313</v>
+      </c>
+      <c r="G225" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A226" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B226" t="s">
+        <v>326</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="F226" t="s">
+        <v>313</v>
+      </c>
+      <c r="G226" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A227" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B227" t="s">
+        <v>327</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
+      </c>
+      <c r="F227" t="s">
+        <v>313</v>
+      </c>
+      <c r="G227" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A228" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B228" t="s">
+        <v>330</v>
+      </c>
+      <c r="E228">
+        <v>2</v>
+      </c>
+      <c r="F228" t="s">
+        <v>313</v>
+      </c>
+      <c r="G228" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A229" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B229" t="s">
+        <v>328</v>
+      </c>
+      <c r="E229">
+        <v>2</v>
+      </c>
+      <c r="F229" t="s">
+        <v>313</v>
+      </c>
+      <c r="G229" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A230" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B230" t="s">
+        <v>329</v>
+      </c>
+      <c r="E230">
+        <v>2</v>
+      </c>
+      <c r="F230" t="s">
+        <v>313</v>
+      </c>
+      <c r="G230" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on funda factors
</commit_message>
<xml_diff>
--- a/config/factorTable2023.xlsx
+++ b/config/factorTable2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramFiles\python\strategy_factor\BigMom2023\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD807E83-C3EE-4695-9CB2-B8DFABC8C11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C01E486-1A8B-4CB5-A5E7-C08D012171F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="3225" windowWidth="19305" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40425" yWindow="5565" windowWidth="21330" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="344">
   <si>
     <t>formula</t>
   </si>
@@ -1295,35 +1295,50 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>str('D:/Data/tushare/factor/main_sub_spread.csv');list((5,20,60,90,120));list((1,5,10,15,21))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/oi_all.csv');list((5,20,60,90,120));list((1,5,10,15,22))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_rate.csv');list((5,20,60,90,120));list((1,5,10,15,23))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,24))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,25))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_w_rate.csv');list((5,20,60,90,120));list((1,5,10,15,24))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_w_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,25))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str('D:/Data/tushare/factor/fut_w_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,26))</t>
+    <t>alpha_f10</t>
+  </si>
+  <si>
+    <t>main_sub_spread_diff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kdj</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/main_sub_spread.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/oi_all.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate5.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/fut_w_rate10.csv');list((5,20,60,90,120));list((1,5,10,15,20))</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>str('D:/Data/tushare/factor/main_sub_spread.csv');list((1,3,5,10,20));list((1,5,10,15,20))</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1331,11 +1346,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1343,13 +1358,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1427,9 +1442,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1467,9 +1482,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1502,26 +1517,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1554,26 +1552,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1747,26 +1728,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H230"/>
+  <dimension ref="A1:H231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G230" sqref="G230"/>
+      <selection pane="bottomRight" activeCell="G232" sqref="G232"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="86.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.25" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="17.875" customWidth="1"/>
+    <col min="7" max="7" width="113.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1792,12 +1775,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1812,12 +1795,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1832,12 +1815,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1852,12 +1835,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1872,12 +1855,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1892,12 +1875,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1912,12 +1895,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1932,12 +1915,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1952,12 +1935,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1972,12 +1955,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1992,12 +1975,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2012,12 +1995,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2032,12 +2015,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2052,12 +2035,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2072,12 +2055,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2092,12 +2075,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2112,12 +2095,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2132,12 +2115,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2152,12 +2135,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2172,12 +2155,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2192,12 +2175,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2212,12 +2195,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>97</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2232,12 +2215,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2252,12 +2235,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2272,12 +2255,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2292,12 +2275,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2312,12 +2295,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2332,12 +2315,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2352,12 +2335,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2372,12 +2355,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2392,12 +2375,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2412,12 +2395,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2432,12 +2415,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2452,12 +2435,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2472,12 +2455,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2492,12 +2475,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2512,12 +2495,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2532,12 +2515,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2552,12 +2535,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2572,12 +2555,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2592,12 +2575,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2612,12 +2595,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2632,12 +2615,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2652,12 +2635,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2672,12 +2655,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2692,12 +2675,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2712,12 +2695,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2732,12 +2715,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2752,12 +2735,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2772,12 +2755,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2792,12 +2775,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2812,12 +2795,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2832,12 +2815,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2852,12 +2835,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2872,12 +2855,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2892,12 +2875,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2912,12 +2895,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2932,12 +2915,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2952,12 +2935,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2972,12 +2955,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2992,12 +2975,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3012,12 +2995,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3032,12 +3015,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3052,12 +3035,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3072,12 +3055,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3092,12 +3075,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3112,12 +3095,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3132,12 +3115,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3152,12 +3135,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -3172,12 +3155,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3192,12 +3175,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3212,12 +3195,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -3232,12 +3215,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3252,12 +3235,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3272,12 +3255,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3292,12 +3275,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3312,12 +3295,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3332,12 +3315,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3352,12 +3335,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3372,12 +3355,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>163</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3392,12 +3375,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3412,12 +3395,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -3432,12 +3415,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3452,12 +3435,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -3472,12 +3455,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3492,12 +3475,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>171</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3512,12 +3495,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3532,12 +3515,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>173</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3552,12 +3535,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>174</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3572,12 +3555,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -3592,12 +3575,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>176</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3612,12 +3595,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -3632,12 +3615,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -3652,12 +3635,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3672,12 +3655,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -3692,12 +3675,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -3712,12 +3695,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
         <v>206</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -3732,12 +3715,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -3752,12 +3735,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -3772,12 +3755,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>311</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -3792,12 +3775,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
         <v>209</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -3812,12 +3795,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
         <v>210</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -3832,12 +3815,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
         <v>211</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -3852,12 +3835,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
         <v>212</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -3872,12 +3855,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
         <v>213</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -3892,12 +3875,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -3912,12 +3895,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
         <v>217</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -3932,12 +3915,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
         <v>218</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -3952,12 +3935,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -3972,12 +3955,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
         <v>220</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -3992,12 +3975,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -4012,12 +3995,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
         <v>222</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -4032,12 +4015,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="12.75" customHeight="1">
+    <row r="114" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
         <v>223</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -4052,12 +4035,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -4072,12 +4055,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="12.75" customHeight="1">
+    <row r="116" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -4092,12 +4075,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
         <v>226</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -4112,12 +4095,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
         <v>228</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -4132,12 +4115,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
         <v>229</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -4152,12 +4135,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
         <v>230</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -4172,12 +4155,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
         <v>231</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -4192,12 +4175,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -4212,12 +4195,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
         <v>233</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -4232,12 +4215,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
         <v>234</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -4252,12 +4235,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
         <v>236</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -4272,12 +4255,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
         <v>237</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -4292,12 +4275,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
         <v>238</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -4312,12 +4295,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -4332,12 +4315,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
         <v>240</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -4352,12 +4335,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
         <v>241</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -4372,12 +4355,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -4392,12 +4375,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="12.75" customHeight="1">
+    <row r="132" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
         <v>243</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -4412,12 +4395,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
         <v>244</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -4432,12 +4415,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -4452,12 +4435,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
         <v>246</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -4472,12 +4455,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="12.75" customHeight="1">
+    <row r="136" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
         <v>247</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D136">
         <v>0</v>
@@ -4492,12 +4475,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -4512,12 +4495,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
         <v>249</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -4532,12 +4515,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -4552,12 +4535,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
         <v>252</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -4572,12 +4555,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
         <v>253</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -4592,12 +4575,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
         <v>254</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -4612,12 +4595,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
         <v>255</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -4632,12 +4615,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
         <v>256</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -4652,12 +4635,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="12.75" customHeight="1">
+    <row r="145" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
         <v>257</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -4672,12 +4655,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
         <v>259</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -4692,12 +4675,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
         <v>260</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -4712,12 +4695,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
         <v>261</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -4732,12 +4715,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
         <v>262</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -4752,12 +4735,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
         <v>264</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -4772,12 +4755,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="12.75" customHeight="1">
+    <row r="151" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
         <v>265</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -4792,12 +4775,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
         <v>267</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -4812,7 +4795,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
         <v>268</v>
       </c>
@@ -4832,12 +4815,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -4852,12 +4835,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -4872,12 +4855,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
         <v>271</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -4892,12 +4875,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
         <v>272</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -4912,12 +4895,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
         <v>273</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -4932,12 +4915,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
         <v>274</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -4952,12 +4935,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="12.75" customHeight="1">
+    <row r="160" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
         <v>275</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -4972,12 +4955,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="12.75" customHeight="1">
+    <row r="161" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
         <v>276</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -4992,12 +4975,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="12.75" customHeight="1">
+    <row r="162" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
         <v>277</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -5012,12 +4995,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
         <v>278</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -5032,12 +5015,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
         <v>279</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D164">
         <v>0</v>
@@ -5052,12 +5035,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
         <v>280</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D165">
         <v>0</v>
@@ -5072,12 +5055,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
         <v>281</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -5092,12 +5075,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
         <v>282</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -5112,12 +5095,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
         <v>283</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D168">
         <v>0</v>
@@ -5132,12 +5115,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
         <v>284</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -5152,12 +5135,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
         <v>285</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -5172,12 +5155,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
         <v>286</v>
       </c>
       <c r="C171">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -5192,12 +5175,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
         <v>287</v>
       </c>
       <c r="C172">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -5212,12 +5195,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
         <v>288</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -5232,12 +5215,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
         <v>289</v>
       </c>
       <c r="C174">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -5252,12 +5235,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
         <v>290</v>
       </c>
       <c r="C175">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -5272,12 +5255,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
         <v>291</v>
       </c>
       <c r="C176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -5292,12 +5275,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
         <v>292</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -5312,12 +5295,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
         <v>293</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -5332,12 +5315,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
         <v>294</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -5352,12 +5335,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -5372,12 +5355,12 @@
         <v>296</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
         <v>297</v>
       </c>
       <c r="C181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -5392,12 +5375,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
         <v>298</v>
       </c>
       <c r="C182">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -5412,12 +5395,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
         <v>299</v>
       </c>
       <c r="C183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -5432,12 +5415,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -5452,12 +5435,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="12.75" customHeight="1">
+    <row r="185" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
         <v>301</v>
       </c>
       <c r="C185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -5472,12 +5455,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
         <v>302</v>
       </c>
       <c r="C186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -5492,12 +5475,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
         <v>303</v>
       </c>
       <c r="C187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -5512,12 +5495,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
         <v>304</v>
       </c>
       <c r="C188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -5532,12 +5515,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
         <v>306</v>
       </c>
       <c r="C189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -5552,12 +5535,12 @@
         <v>305</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
         <v>307</v>
       </c>
       <c r="C190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -5572,12 +5555,12 @@
         <v>305</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="12.75" customHeight="1">
+    <row r="191" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
         <v>308</v>
       </c>
       <c r="C191">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -5592,12 +5575,12 @@
         <v>305</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
         <v>309</v>
       </c>
       <c r="C192">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -5612,7 +5595,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
         <v>2</v>
       </c>
@@ -5620,7 +5603,7 @@
         <v>65</v>
       </c>
       <c r="C193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -5635,7 +5618,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
@@ -5643,7 +5626,7 @@
         <v>30</v>
       </c>
       <c r="C194">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -5658,7 +5641,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
         <v>4</v>
       </c>
@@ -5666,7 +5649,7 @@
         <v>31</v>
       </c>
       <c r="C195">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -5681,7 +5664,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
         <v>5</v>
       </c>
@@ -5689,7 +5672,7 @@
         <v>32</v>
       </c>
       <c r="C196">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -5704,7 +5687,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
         <v>6</v>
       </c>
@@ -5712,7 +5695,7 @@
         <v>33</v>
       </c>
       <c r="C197">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -5727,7 +5710,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="12.75" customHeight="1">
+    <row r="198" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
         <v>7</v>
       </c>
@@ -5735,7 +5718,7 @@
         <v>34</v>
       </c>
       <c r="C198">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -5750,7 +5733,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
         <v>8</v>
       </c>
@@ -5758,7 +5741,7 @@
         <v>35</v>
       </c>
       <c r="C199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -5773,7 +5756,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="12.75" customHeight="1">
+    <row r="200" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
         <v>9</v>
       </c>
@@ -5781,7 +5764,7 @@
         <v>36</v>
       </c>
       <c r="C200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -5796,7 +5779,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="12.75" customHeight="1">
+    <row r="201" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
         <v>10</v>
       </c>
@@ -5804,7 +5787,7 @@
         <v>37</v>
       </c>
       <c r="C201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -5819,7 +5802,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="12.75" customHeight="1">
+    <row r="202" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
         <v>11</v>
       </c>
@@ -5827,7 +5810,7 @@
         <v>38</v>
       </c>
       <c r="C202">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -5842,7 +5825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
         <v>12</v>
       </c>
@@ -5850,7 +5833,7 @@
         <v>39</v>
       </c>
       <c r="C203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -5865,7 +5848,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="12.75" customHeight="1">
+    <row r="204" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
         <v>13</v>
       </c>
@@ -5873,7 +5856,7 @@
         <v>40</v>
       </c>
       <c r="C204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -5888,7 +5871,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="12.75" customHeight="1">
+    <row r="205" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
         <v>14</v>
       </c>
@@ -5896,7 +5879,7 @@
         <v>41</v>
       </c>
       <c r="C205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -5911,7 +5894,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="12.75" customHeight="1">
+    <row r="206" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
         <v>15</v>
       </c>
@@ -5919,7 +5902,7 @@
         <v>42</v>
       </c>
       <c r="C206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -5934,7 +5917,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
         <v>16</v>
       </c>
@@ -5942,7 +5925,7 @@
         <v>43</v>
       </c>
       <c r="C207">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -5957,7 +5940,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="12.75" customHeight="1">
+    <row r="208" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
         <v>17</v>
       </c>
@@ -5965,7 +5948,7 @@
         <v>44</v>
       </c>
       <c r="C208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -5980,7 +5963,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
         <v>18</v>
       </c>
@@ -5988,7 +5971,7 @@
         <v>45</v>
       </c>
       <c r="C209">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -6003,7 +5986,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="12.75" customHeight="1">
+    <row r="210" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
         <v>19</v>
       </c>
@@ -6011,7 +5994,7 @@
         <v>46</v>
       </c>
       <c r="C210">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -6026,7 +6009,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="12.75" customHeight="1">
+    <row r="211" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A211" s="1" t="s">
         <v>20</v>
       </c>
@@ -6034,7 +6017,7 @@
         <v>47</v>
       </c>
       <c r="C211">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D211">
         <v>0</v>
@@ -6049,7 +6032,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="12.75" customHeight="1">
+    <row r="212" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
         <v>21</v>
       </c>
@@ -6057,7 +6040,7 @@
         <v>48</v>
       </c>
       <c r="C212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D212">
         <v>0</v>
@@ -6072,7 +6055,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="12.75" customHeight="1">
+    <row r="213" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
         <v>22</v>
       </c>
@@ -6080,7 +6063,7 @@
         <v>49</v>
       </c>
       <c r="C213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -6095,7 +6078,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="12.75" customHeight="1">
+    <row r="214" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
         <v>23</v>
       </c>
@@ -6103,7 +6086,7 @@
         <v>50</v>
       </c>
       <c r="C214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D214">
         <v>0</v>
@@ -6118,7 +6101,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="12.75" customHeight="1">
+    <row r="215" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
         <v>24</v>
       </c>
@@ -6126,7 +6109,7 @@
         <v>51</v>
       </c>
       <c r="C215">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D215">
         <v>0</v>
@@ -6141,7 +6124,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="12.75" customHeight="1">
+    <row r="216" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
         <v>25</v>
       </c>
@@ -6149,7 +6132,7 @@
         <v>52</v>
       </c>
       <c r="C216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D216">
         <v>0</v>
@@ -6164,7 +6147,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="12.75" customHeight="1">
+    <row r="217" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
         <v>26</v>
       </c>
@@ -6172,7 +6155,7 @@
         <v>53</v>
       </c>
       <c r="C217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -6187,7 +6170,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="12.75" customHeight="1">
+    <row r="218" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
         <v>27</v>
       </c>
@@ -6195,7 +6178,7 @@
         <v>54</v>
       </c>
       <c r="C218">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D218">
         <v>0</v>
@@ -6210,7 +6193,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="12.75" customHeight="1">
+    <row r="219" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
         <v>28</v>
       </c>
@@ -6218,7 +6201,7 @@
         <v>61</v>
       </c>
       <c r="C219">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D219">
         <v>0</v>
@@ -6233,7 +6216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="12.75" customHeight="1">
+    <row r="220" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
         <v>29</v>
       </c>
@@ -6241,7 +6224,7 @@
         <v>60</v>
       </c>
       <c r="C220">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D220">
         <v>0</v>
@@ -6256,12 +6239,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="12.75" customHeight="1">
+    <row r="221" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B221" t="s">
+        <v>334</v>
+      </c>
       <c r="C221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D221">
         <v>0</v>
@@ -6276,13 +6262,19 @@
         <v>84</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A222" s="2" t="s">
         <v>312</v>
       </c>
       <c r="B222" t="s">
         <v>322</v>
       </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
       <c r="E222">
         <v>2</v>
       </c>
@@ -6293,13 +6285,19 @@
         <v>331</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A223" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B223" t="s">
         <v>323</v>
       </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
       <c r="E223">
         <v>2</v>
       </c>
@@ -6307,16 +6305,22 @@
         <v>313</v>
       </c>
       <c r="G223" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="224" spans="1:7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A224" s="2" t="s">
         <v>315</v>
       </c>
       <c r="B224" t="s">
         <v>324</v>
       </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
       <c r="E224">
         <v>2</v>
       </c>
@@ -6324,16 +6328,22 @@
         <v>313</v>
       </c>
       <c r="G224" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A225" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B225" t="s">
         <v>325</v>
       </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
       <c r="E225">
         <v>2</v>
       </c>
@@ -6341,16 +6351,22 @@
         <v>313</v>
       </c>
       <c r="G225" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A226" s="2" t="s">
         <v>317</v>
       </c>
       <c r="B226" t="s">
         <v>326</v>
       </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
       <c r="E226">
         <v>2</v>
       </c>
@@ -6358,16 +6374,22 @@
         <v>313</v>
       </c>
       <c r="G226" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A227" s="2" t="s">
         <v>318</v>
       </c>
       <c r="B227" t="s">
         <v>327</v>
       </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
       <c r="E227">
         <v>2</v>
       </c>
@@ -6375,16 +6397,22 @@
         <v>313</v>
       </c>
       <c r="G227" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A228" s="2" t="s">
         <v>319</v>
       </c>
       <c r="B228" t="s">
         <v>330</v>
       </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
       <c r="E228">
         <v>2</v>
       </c>
@@ -6392,16 +6420,22 @@
         <v>313</v>
       </c>
       <c r="G228" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A229" s="2" t="s">
         <v>320</v>
       </c>
       <c r="B229" t="s">
         <v>328</v>
       </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
       <c r="E229">
         <v>2</v>
       </c>
@@ -6409,16 +6443,22 @@
         <v>313</v>
       </c>
       <c r="G229" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="230" spans="1:7">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A230" s="2" t="s">
         <v>321</v>
       </c>
       <c r="B230" t="s">
         <v>329</v>
       </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
       <c r="E230">
         <v>2</v>
       </c>
@@ -6426,7 +6466,27 @@
         <v>313</v>
       </c>
       <c r="G230" t="s">
-        <v>339</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A231" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B231" t="s">
+        <v>333</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="F231" t="s">
+        <v>313</v>
+      </c>
+      <c r="G231" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>